<commit_message>
Crear estructura de archivos del proyecto para acceder a las vistas y agregar las rutas respectivas para acceder a cada una. Crear vista de home de mediateca. Crear vista de grados de telesecundaria . Crear vista de semestres de telebachillerato.
</commit_message>
<xml_diff>
--- a/public/imagenes/mediateca/Asignaturas Telesecundaria.xlsx
+++ b/public/imagenes/mediateca/Asignaturas Telesecundaria.xlsx
@@ -1232,335 +1232,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image01.png"/>
+        <xdr:cNvPr id="0" name="image00.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:ext cx="209550" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>